<commit_message>
all data cleaning ready
</commit_message>
<xml_diff>
--- a/docs/panel_comparison.xlsx
+++ b/docs/panel_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\tesis_cyv\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00589C1E-D9D5-4636-B127-FEC0918EFCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833D05D3-F44D-401F-A4C6-B5726E83C449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2490" windowWidth="29040" windowHeight="15720" xr2:uid="{0D8AFCBD-9317-4E52-8EEE-06421CBD2BDB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0D8AFCBD-9317-4E52-8EEE-06421CBD2BDB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="526">
   <si>
     <t>Variable</t>
   </si>
@@ -590,7 +590,1030 @@
     <t>Modulo 500 (base)</t>
   </si>
   <si>
-    <t>creada</t>
+    <t>p101_18</t>
+  </si>
+  <si>
+    <t>p102_18</t>
+  </si>
+  <si>
+    <t>p103_18</t>
+  </si>
+  <si>
+    <t>p103a_18</t>
+  </si>
+  <si>
+    <t>p104_18</t>
+  </si>
+  <si>
+    <t>p104a_18</t>
+  </si>
+  <si>
+    <t>p105a_18</t>
+  </si>
+  <si>
+    <t>p105b_18</t>
+  </si>
+  <si>
+    <t>p106_18</t>
+  </si>
+  <si>
+    <t>p106b_18</t>
+  </si>
+  <si>
+    <t>p107b1_18</t>
+  </si>
+  <si>
+    <t>p110_18</t>
+  </si>
+  <si>
+    <t>p110a1_18</t>
+  </si>
+  <si>
+    <t>p110c_18</t>
+  </si>
+  <si>
+    <t>p111a_18</t>
+  </si>
+  <si>
+    <t>p112a_18</t>
+  </si>
+  <si>
+    <t>p1142_18</t>
+  </si>
+  <si>
+    <t>p1144_18</t>
+  </si>
+  <si>
+    <t>p401f_18</t>
+  </si>
+  <si>
+    <t>p401g1_18</t>
+  </si>
+  <si>
+    <t>p401_18</t>
+  </si>
+  <si>
+    <t>p4021_18</t>
+  </si>
+  <si>
+    <t>p4022_18</t>
+  </si>
+  <si>
+    <t>p4023_18</t>
+  </si>
+  <si>
+    <t>p4024_18</t>
+  </si>
+  <si>
+    <t>p4025_18</t>
+  </si>
+  <si>
+    <t>p4191_18</t>
+  </si>
+  <si>
+    <t>p4192_18</t>
+  </si>
+  <si>
+    <t>p4193_18</t>
+  </si>
+  <si>
+    <t>p4194_18</t>
+  </si>
+  <si>
+    <t>p4195_18</t>
+  </si>
+  <si>
+    <t>p4196_18</t>
+  </si>
+  <si>
+    <t>p4197_18</t>
+  </si>
+  <si>
+    <t>p4198_18</t>
+  </si>
+  <si>
+    <t>p300a_18</t>
+  </si>
+  <si>
+    <t>p301a_18</t>
+  </si>
+  <si>
+    <t>p302_18</t>
+  </si>
+  <si>
+    <t>p313_18</t>
+  </si>
+  <si>
+    <t>p314a_18</t>
+  </si>
+  <si>
+    <t>p316b_18</t>
+  </si>
+  <si>
+    <t>p501_18</t>
+  </si>
+  <si>
+    <t>p507_18</t>
+  </si>
+  <si>
+    <t>p510_18</t>
+  </si>
+  <si>
+    <t>p510a1_18</t>
+  </si>
+  <si>
+    <t>p510b_18</t>
+  </si>
+  <si>
+    <t>p511a_18</t>
+  </si>
+  <si>
+    <t>p512a_18</t>
+  </si>
+  <si>
+    <t>p513t_18</t>
+  </si>
+  <si>
+    <t>p513a1_18</t>
+  </si>
+  <si>
+    <t>p513a2_18</t>
+  </si>
+  <si>
+    <t>p514_18</t>
+  </si>
+  <si>
+    <t>p519_18</t>
+  </si>
+  <si>
+    <t>p520_18</t>
+  </si>
+  <si>
+    <t>p521a_18</t>
+  </si>
+  <si>
+    <t>p521c_18</t>
+  </si>
+  <si>
+    <t>p524a1_18</t>
+  </si>
+  <si>
+    <t>p524a2_18</t>
+  </si>
+  <si>
+    <t>p528_18</t>
+  </si>
+  <si>
+    <t>p530a_18</t>
+  </si>
+  <si>
+    <t>p530b_18</t>
+  </si>
+  <si>
+    <t>p535_18</t>
+  </si>
+  <si>
+    <t>p558c_18</t>
+  </si>
+  <si>
+    <t>p558d_18</t>
+  </si>
+  <si>
+    <t>p207_18</t>
+  </si>
+  <si>
+    <t>p208a_18</t>
+  </si>
+  <si>
+    <t>p209_18</t>
+  </si>
+  <si>
+    <t>conglome_18</t>
+  </si>
+  <si>
+    <t>vivienda_18</t>
+  </si>
+  <si>
+    <t>hogar_18</t>
+  </si>
+  <si>
+    <t>codperso_18</t>
+  </si>
+  <si>
+    <t>creada a partir de ocupinf</t>
+  </si>
+  <si>
+    <t>percepho_18</t>
+  </si>
+  <si>
+    <t>mieperho_18</t>
+  </si>
+  <si>
+    <t>ingbruhd_18</t>
+  </si>
+  <si>
+    <t>ingindhd_18</t>
+  </si>
+  <si>
+    <t>insedthd_18</t>
+  </si>
+  <si>
+    <t>ingseihd_18</t>
+  </si>
+  <si>
+    <t>ingexthd_18</t>
+  </si>
+  <si>
+    <t>ingtrahd_18</t>
+  </si>
+  <si>
+    <t>ingtexhd_18</t>
+  </si>
+  <si>
+    <t>ingrenhd_18</t>
+  </si>
+  <si>
+    <t>ingmo1hd_18</t>
+  </si>
+  <si>
+    <t>inghog1d_18</t>
+  </si>
+  <si>
+    <t>gashog1d_18</t>
+  </si>
+  <si>
+    <t>estrsocial_18</t>
+  </si>
+  <si>
+    <t>linea_18</t>
+  </si>
+  <si>
+    <t>pobreza_18</t>
+  </si>
+  <si>
+    <t>p207_17</t>
+  </si>
+  <si>
+    <t>p208a_17</t>
+  </si>
+  <si>
+    <t>p209_17</t>
+  </si>
+  <si>
+    <t>p303_19</t>
+  </si>
+  <si>
+    <t>p303_18</t>
+  </si>
+  <si>
+    <t>conglome_17</t>
+  </si>
+  <si>
+    <t>vivienda_17</t>
+  </si>
+  <si>
+    <t>hogar_17</t>
+  </si>
+  <si>
+    <t>codperso_17</t>
+  </si>
+  <si>
+    <t>p501_17</t>
+  </si>
+  <si>
+    <t>p507_17</t>
+  </si>
+  <si>
+    <t>p510_17</t>
+  </si>
+  <si>
+    <t>p510a1_17</t>
+  </si>
+  <si>
+    <t>p510b_17</t>
+  </si>
+  <si>
+    <t>p511a_17</t>
+  </si>
+  <si>
+    <t>p512a_17</t>
+  </si>
+  <si>
+    <t>p513t_17</t>
+  </si>
+  <si>
+    <t>p513a1_17</t>
+  </si>
+  <si>
+    <t>p513a2_17</t>
+  </si>
+  <si>
+    <t>p514_17</t>
+  </si>
+  <si>
+    <t>p519_17</t>
+  </si>
+  <si>
+    <t>p520_17</t>
+  </si>
+  <si>
+    <t>p521a_17</t>
+  </si>
+  <si>
+    <t>p521c_17</t>
+  </si>
+  <si>
+    <t>p524a1_17</t>
+  </si>
+  <si>
+    <t>p524a2_17</t>
+  </si>
+  <si>
+    <t>p528_17</t>
+  </si>
+  <si>
+    <t>p530a_17</t>
+  </si>
+  <si>
+    <t>p530b_17</t>
+  </si>
+  <si>
+    <t>p535_17</t>
+  </si>
+  <si>
+    <t>p558c_17</t>
+  </si>
+  <si>
+    <t>p558d_17</t>
+  </si>
+  <si>
+    <t>p300a_17</t>
+  </si>
+  <si>
+    <t>p301a_17</t>
+  </si>
+  <si>
+    <t>p302_17</t>
+  </si>
+  <si>
+    <t>p303_17</t>
+  </si>
+  <si>
+    <t>p313_17</t>
+  </si>
+  <si>
+    <t>p314a_17</t>
+  </si>
+  <si>
+    <t>p401f_17</t>
+  </si>
+  <si>
+    <t>p401_17</t>
+  </si>
+  <si>
+    <t>p4021_17</t>
+  </si>
+  <si>
+    <t>p4022_17</t>
+  </si>
+  <si>
+    <t>p4023_17</t>
+  </si>
+  <si>
+    <t>p4024_17</t>
+  </si>
+  <si>
+    <t>p4025_17</t>
+  </si>
+  <si>
+    <t>p4191_17</t>
+  </si>
+  <si>
+    <t>p4192_17</t>
+  </si>
+  <si>
+    <t>p4193_17</t>
+  </si>
+  <si>
+    <t>p4194_17</t>
+  </si>
+  <si>
+    <t>p4195_17</t>
+  </si>
+  <si>
+    <t>p4196_17</t>
+  </si>
+  <si>
+    <t>p4197_17</t>
+  </si>
+  <si>
+    <t>p4198_17</t>
+  </si>
+  <si>
+    <t>p101_17</t>
+  </si>
+  <si>
+    <t>p102_17</t>
+  </si>
+  <si>
+    <t>p103_17</t>
+  </si>
+  <si>
+    <t>p103a_17</t>
+  </si>
+  <si>
+    <t>p104_17</t>
+  </si>
+  <si>
+    <t>p104a_17</t>
+  </si>
+  <si>
+    <t>p105a_17</t>
+  </si>
+  <si>
+    <t>p105b_17</t>
+  </si>
+  <si>
+    <t>p106_17</t>
+  </si>
+  <si>
+    <t>p106b_17</t>
+  </si>
+  <si>
+    <t>p107b1_17</t>
+  </si>
+  <si>
+    <t>p110_17</t>
+  </si>
+  <si>
+    <t>p110a1_17</t>
+  </si>
+  <si>
+    <t>p110c_17</t>
+  </si>
+  <si>
+    <t>p111a_17</t>
+  </si>
+  <si>
+    <t>p112a_17</t>
+  </si>
+  <si>
+    <t>p1142_17</t>
+  </si>
+  <si>
+    <t>p1144_17</t>
+  </si>
+  <si>
+    <t>percepho_17</t>
+  </si>
+  <si>
+    <t>mieperho_17</t>
+  </si>
+  <si>
+    <t>ingbruhd_17</t>
+  </si>
+  <si>
+    <t>ingindhd_17</t>
+  </si>
+  <si>
+    <t>insedthd_17</t>
+  </si>
+  <si>
+    <t>ingseihd_17</t>
+  </si>
+  <si>
+    <t>ingexthd_17</t>
+  </si>
+  <si>
+    <t>ingtrahd_17</t>
+  </si>
+  <si>
+    <t>ingtexhd_17</t>
+  </si>
+  <si>
+    <t>ingrenhd_17</t>
+  </si>
+  <si>
+    <t>ingmo1hd_17</t>
+  </si>
+  <si>
+    <t>inghog1d_17</t>
+  </si>
+  <si>
+    <t>gashog1d_17</t>
+  </si>
+  <si>
+    <t>estrsocial_17</t>
+  </si>
+  <si>
+    <t>linea_17</t>
+  </si>
+  <si>
+    <t>pobreza_17</t>
+  </si>
+  <si>
+    <t>conglome_16</t>
+  </si>
+  <si>
+    <t>vivienda_16</t>
+  </si>
+  <si>
+    <t>hogar_16</t>
+  </si>
+  <si>
+    <t>codperso_16</t>
+  </si>
+  <si>
+    <t>p207_16</t>
+  </si>
+  <si>
+    <t>p208a_16</t>
+  </si>
+  <si>
+    <t>p209_16</t>
+  </si>
+  <si>
+    <t>p501_16</t>
+  </si>
+  <si>
+    <t>p507_16</t>
+  </si>
+  <si>
+    <t>p510_16</t>
+  </si>
+  <si>
+    <t>p510a1_16</t>
+  </si>
+  <si>
+    <t>p510b_16</t>
+  </si>
+  <si>
+    <t>p511a_16</t>
+  </si>
+  <si>
+    <t>p512a_16</t>
+  </si>
+  <si>
+    <t>p513t_16</t>
+  </si>
+  <si>
+    <t>p513a1_16</t>
+  </si>
+  <si>
+    <t>p513a2_16</t>
+  </si>
+  <si>
+    <t>p514_16</t>
+  </si>
+  <si>
+    <t>p519_16</t>
+  </si>
+  <si>
+    <t>p520_16</t>
+  </si>
+  <si>
+    <t>p521a_16</t>
+  </si>
+  <si>
+    <t>p521c_16</t>
+  </si>
+  <si>
+    <t>p524a1_16</t>
+  </si>
+  <si>
+    <t>p524a2_16</t>
+  </si>
+  <si>
+    <t>p528_16</t>
+  </si>
+  <si>
+    <t>p530a_16</t>
+  </si>
+  <si>
+    <t>p530b_16</t>
+  </si>
+  <si>
+    <t>p535_16</t>
+  </si>
+  <si>
+    <t>p558c_16</t>
+  </si>
+  <si>
+    <t>p558d_16</t>
+  </si>
+  <si>
+    <t>p300a_16</t>
+  </si>
+  <si>
+    <t>p301a_16</t>
+  </si>
+  <si>
+    <t>p302_16</t>
+  </si>
+  <si>
+    <t>p303_16</t>
+  </si>
+  <si>
+    <t>p313_16</t>
+  </si>
+  <si>
+    <t>p314a_16</t>
+  </si>
+  <si>
+    <t>p401f_16</t>
+  </si>
+  <si>
+    <t>p401_16</t>
+  </si>
+  <si>
+    <t>p4021_16</t>
+  </si>
+  <si>
+    <t>p4022_16</t>
+  </si>
+  <si>
+    <t>p4023_16</t>
+  </si>
+  <si>
+    <t>p4024_16</t>
+  </si>
+  <si>
+    <t>p4025_16</t>
+  </si>
+  <si>
+    <t>p4191_16</t>
+  </si>
+  <si>
+    <t>p4192_16</t>
+  </si>
+  <si>
+    <t>p4193_16</t>
+  </si>
+  <si>
+    <t>p4194_16</t>
+  </si>
+  <si>
+    <t>p4195_16</t>
+  </si>
+  <si>
+    <t>p4196_16</t>
+  </si>
+  <si>
+    <t>p4197_16</t>
+  </si>
+  <si>
+    <t>p4198_16</t>
+  </si>
+  <si>
+    <t>p101_16</t>
+  </si>
+  <si>
+    <t>p102_16</t>
+  </si>
+  <si>
+    <t>p103_16</t>
+  </si>
+  <si>
+    <t>p103a_16</t>
+  </si>
+  <si>
+    <t>p104_16</t>
+  </si>
+  <si>
+    <t>p104a_16</t>
+  </si>
+  <si>
+    <t>p105a_16</t>
+  </si>
+  <si>
+    <t>p105b_16</t>
+  </si>
+  <si>
+    <t>p106_16</t>
+  </si>
+  <si>
+    <t>p106b_16</t>
+  </si>
+  <si>
+    <t>p107b1_16</t>
+  </si>
+  <si>
+    <t>p110_16</t>
+  </si>
+  <si>
+    <t>p110a1_16</t>
+  </si>
+  <si>
+    <t>p111a_16</t>
+  </si>
+  <si>
+    <t>p112a_16</t>
+  </si>
+  <si>
+    <t>p1142_16</t>
+  </si>
+  <si>
+    <t>p1144_16</t>
+  </si>
+  <si>
+    <t>percepho_16</t>
+  </si>
+  <si>
+    <t>mieperho_16</t>
+  </si>
+  <si>
+    <t>ingbruhd_16</t>
+  </si>
+  <si>
+    <t>ingindhd_16</t>
+  </si>
+  <si>
+    <t>insedthd_16</t>
+  </si>
+  <si>
+    <t>ingseihd_16</t>
+  </si>
+  <si>
+    <t>ingexthd_16</t>
+  </si>
+  <si>
+    <t>ingtrahd_16</t>
+  </si>
+  <si>
+    <t>ingtexhd_16</t>
+  </si>
+  <si>
+    <t>ingrenhd_16</t>
+  </si>
+  <si>
+    <t>ingmo1hd_16</t>
+  </si>
+  <si>
+    <t>inghog1d_16</t>
+  </si>
+  <si>
+    <t>gashog1d_16</t>
+  </si>
+  <si>
+    <t>estrsocial_16</t>
+  </si>
+  <si>
+    <t>linea_16</t>
+  </si>
+  <si>
+    <t>pobreza_16</t>
+  </si>
+  <si>
+    <t>conglome_15</t>
+  </si>
+  <si>
+    <t>vivienda_15</t>
+  </si>
+  <si>
+    <t>hogar_15</t>
+  </si>
+  <si>
+    <t>codperso_15</t>
+  </si>
+  <si>
+    <t>p207_15</t>
+  </si>
+  <si>
+    <t>p208a_15</t>
+  </si>
+  <si>
+    <t>p209_15</t>
+  </si>
+  <si>
+    <t>p501_15</t>
+  </si>
+  <si>
+    <t>p507_15</t>
+  </si>
+  <si>
+    <t>p510_15</t>
+  </si>
+  <si>
+    <t>p510a1_15</t>
+  </si>
+  <si>
+    <t>p510b_15</t>
+  </si>
+  <si>
+    <t>p511a_15</t>
+  </si>
+  <si>
+    <t>p512a_15</t>
+  </si>
+  <si>
+    <t>p513t_15</t>
+  </si>
+  <si>
+    <t>p513a1_15</t>
+  </si>
+  <si>
+    <t>p513a2_15</t>
+  </si>
+  <si>
+    <t>p514_15</t>
+  </si>
+  <si>
+    <t>p519_15</t>
+  </si>
+  <si>
+    <t>p520_15</t>
+  </si>
+  <si>
+    <t>p521a_15</t>
+  </si>
+  <si>
+    <t>p521c_15</t>
+  </si>
+  <si>
+    <t>p524a1_15</t>
+  </si>
+  <si>
+    <t>p524a2_15</t>
+  </si>
+  <si>
+    <t>p528_15</t>
+  </si>
+  <si>
+    <t>p530a_15</t>
+  </si>
+  <si>
+    <t>p530b_15</t>
+  </si>
+  <si>
+    <t>p535_15</t>
+  </si>
+  <si>
+    <t>p558c_15</t>
+  </si>
+  <si>
+    <t>p558d_15</t>
+  </si>
+  <si>
+    <t>p300a_15</t>
+  </si>
+  <si>
+    <t>p301a_15</t>
+  </si>
+  <si>
+    <t>p302_15</t>
+  </si>
+  <si>
+    <t>p303_15</t>
+  </si>
+  <si>
+    <t>p313_15</t>
+  </si>
+  <si>
+    <t>p314a_15</t>
+  </si>
+  <si>
+    <t>p401f_15</t>
+  </si>
+  <si>
+    <t>p401_15</t>
+  </si>
+  <si>
+    <t>p4021_15</t>
+  </si>
+  <si>
+    <t>p4022_15</t>
+  </si>
+  <si>
+    <t>p4023_15</t>
+  </si>
+  <si>
+    <t>p4024_15</t>
+  </si>
+  <si>
+    <t>p4025_15</t>
+  </si>
+  <si>
+    <t>p4191_15</t>
+  </si>
+  <si>
+    <t>p4192_15</t>
+  </si>
+  <si>
+    <t>p4193_15</t>
+  </si>
+  <si>
+    <t>p4194_15</t>
+  </si>
+  <si>
+    <t>p4195_15</t>
+  </si>
+  <si>
+    <t>p4196_15</t>
+  </si>
+  <si>
+    <t>p4197_15</t>
+  </si>
+  <si>
+    <t>p4198_15</t>
+  </si>
+  <si>
+    <t>p101_15</t>
+  </si>
+  <si>
+    <t>p102_15</t>
+  </si>
+  <si>
+    <t>p103_15</t>
+  </si>
+  <si>
+    <t>p103a_15</t>
+  </si>
+  <si>
+    <t>p104_15</t>
+  </si>
+  <si>
+    <t>p104a_15</t>
+  </si>
+  <si>
+    <t>p105a_15</t>
+  </si>
+  <si>
+    <t>p105b_15</t>
+  </si>
+  <si>
+    <t>p106_15</t>
+  </si>
+  <si>
+    <t>p106b_15</t>
+  </si>
+  <si>
+    <t>p107b1_15</t>
+  </si>
+  <si>
+    <t>p110_15</t>
+  </si>
+  <si>
+    <t>p110a1_15</t>
+  </si>
+  <si>
+    <t>p111a_15</t>
+  </si>
+  <si>
+    <t>p112a_15</t>
+  </si>
+  <si>
+    <t>p1142_15</t>
+  </si>
+  <si>
+    <t>p1144_15</t>
+  </si>
+  <si>
+    <t>percepho_15</t>
+  </si>
+  <si>
+    <t>mieperho_15</t>
+  </si>
+  <si>
+    <t>ingbruhd_15</t>
+  </si>
+  <si>
+    <t>ingindhd_15</t>
+  </si>
+  <si>
+    <t>insedthd_15</t>
+  </si>
+  <si>
+    <t>ingseihd_15</t>
+  </si>
+  <si>
+    <t>ingexthd_15</t>
+  </si>
+  <si>
+    <t>ingtrahd_15</t>
+  </si>
+  <si>
+    <t>ingtexhd_15</t>
+  </si>
+  <si>
+    <t>ingrenhd_15</t>
+  </si>
+  <si>
+    <t>ingmo1hd_15</t>
+  </si>
+  <si>
+    <t>inghog1d_15</t>
+  </si>
+  <si>
+    <t>gashog1d_15</t>
+  </si>
+  <si>
+    <t>estrsocial_15</t>
+  </si>
+  <si>
+    <t>linea_15</t>
+  </si>
+  <si>
+    <t>pobreza_15</t>
   </si>
 </sst>
 </file>
@@ -629,7 +1652,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -645,6 +1668,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -689,7 +1718,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -702,6 +1731,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1052,8 +2082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE1F47D-D58C-4138-A233-D19EFA101348}">
   <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,14 +2096,14 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
@@ -1103,7 +2133,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="11" t="s">
         <v>183</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1113,16 +2143,18 @@
         <v>168</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="E3" s="2"/>
+        <v>254</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>254</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1132,14 +2164,24 @@
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
+      <c r="A5" s="10"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1149,14 +2191,24 @@
       <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="9"/>
+      <c r="A6" s="10"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1166,14 +2218,24 @@
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>444</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1183,14 +2245,24 @@
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>445</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>182</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1202,14 +2274,24 @@
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>446</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1219,14 +2301,24 @@
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1236,14 +2328,24 @@
       <c r="D10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>181</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1255,14 +2357,24 @@
       <c r="D11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>449</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1272,14 +2384,24 @@
       <c r="D12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>450</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1289,14 +2411,24 @@
       <c r="D13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1306,14 +2438,24 @@
       <c r="D14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>452</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -1323,14 +2465,24 @@
       <c r="D15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>453</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1340,14 +2492,24 @@
       <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="2" t="s">
         <v>28</v>
       </c>
@@ -1357,14 +2519,24 @@
       <c r="D17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
@@ -1374,14 +2546,24 @@
       <c r="D18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="10"/>
       <c r="B19" s="2" t="s">
         <v>32</v>
       </c>
@@ -1391,14 +2573,24 @@
       <c r="D19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="10"/>
       <c r="B20" s="2" t="s">
         <v>34</v>
       </c>
@@ -1408,14 +2600,24 @@
       <c r="D20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="10"/>
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -1425,14 +2627,24 @@
       <c r="D21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+      <c r="E21" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="10"/>
       <c r="B22" s="2" t="s">
         <v>38</v>
       </c>
@@ -1442,14 +2654,24 @@
       <c r="D22" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="10"/>
       <c r="B23" s="2" t="s">
         <v>40</v>
       </c>
@@ -1459,14 +2681,24 @@
       <c r="D23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="10"/>
       <c r="B24" s="2" t="s">
         <v>42</v>
       </c>
@@ -1476,14 +2708,24 @@
       <c r="D24" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="10"/>
       <c r="B25" s="2" t="s">
         <v>44</v>
       </c>
@@ -1493,14 +2735,24 @@
       <c r="D25" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="10"/>
       <c r="B26" s="2" t="s">
         <v>46</v>
       </c>
@@ -1510,14 +2762,24 @@
       <c r="D26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="10"/>
       <c r="B27" s="2" t="s">
         <v>48</v>
       </c>
@@ -1527,14 +2789,24 @@
       <c r="D27" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="10"/>
       <c r="B28" s="2" t="s">
         <v>49</v>
       </c>
@@ -1544,14 +2816,24 @@
       <c r="D28" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="10"/>
       <c r="B29" s="2" t="s">
         <v>51</v>
       </c>
@@ -1561,14 +2843,24 @@
       <c r="D29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
+      <c r="E29" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="10"/>
       <c r="B30" s="2" t="s">
         <v>53</v>
       </c>
@@ -1578,14 +2870,24 @@
       <c r="D30" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="2" t="s">
         <v>55</v>
       </c>
@@ -1595,14 +2897,24 @@
       <c r="D31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="2" t="s">
         <v>57</v>
       </c>
@@ -1612,14 +2924,24 @@
       <c r="D32" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="2" t="s">
         <v>59</v>
       </c>
@@ -1629,14 +2951,24 @@
       <c r="D33" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>471</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="10" t="s">
         <v>180</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1648,14 +2980,24 @@
       <c r="D34" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
+      <c r="E34" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="2" t="s">
         <v>63</v>
       </c>
@@ -1665,14 +3007,24 @@
       <c r="D35" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
+      <c r="E35" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="2" t="s">
         <v>65</v>
       </c>
@@ -1682,14 +3034,24 @@
       <c r="D36" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="2" t="s">
         <v>67</v>
       </c>
@@ -1697,16 +3059,26 @@
         <v>68</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
+        <v>274</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
+      <c r="A38" s="10"/>
       <c r="B38" s="2" t="s">
         <v>69</v>
       </c>
@@ -1716,14 +3088,24 @@
       <c r="D38" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="9"/>
+      <c r="A39" s="10"/>
       <c r="B39" s="2" t="s">
         <v>71</v>
       </c>
@@ -1733,14 +3115,24 @@
       <c r="D39" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
+      <c r="A40" s="10"/>
       <c r="B40" s="2" t="s">
         <v>73</v>
       </c>
@@ -1750,14 +3142,16 @@
       <c r="D40" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="F40" s="8"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="10" t="s">
         <v>179</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1769,14 +3163,24 @@
       <c r="D41" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>478</v>
+      </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="9"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="2" t="s">
         <v>77</v>
       </c>
@@ -1786,14 +3190,16 @@
       <c r="D42" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="F42" s="8"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="9"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="2" t="s">
         <v>79</v>
       </c>
@@ -1803,14 +3209,24 @@
       <c r="D43" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
+      <c r="E43" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="9"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="2" t="s">
         <v>81</v>
       </c>
@@ -1820,14 +3236,24 @@
       <c r="D44" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
+      <c r="E44" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="9"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="2" t="s">
         <v>83</v>
       </c>
@@ -1837,14 +3263,24 @@
       <c r="D45" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
+      <c r="E45" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="9"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="2" t="s">
         <v>85</v>
       </c>
@@ -1854,14 +3290,24 @@
       <c r="D46" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
+      <c r="E46" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="9"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="2" t="s">
         <v>87</v>
       </c>
@@ -1871,14 +3317,24 @@
       <c r="D47" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
+      <c r="E47" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="9"/>
+      <c r="A48" s="10"/>
       <c r="B48" s="2" t="s">
         <v>89</v>
       </c>
@@ -1888,14 +3344,24 @@
       <c r="D48" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
+      <c r="E48" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>484</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="9"/>
+      <c r="A49" s="10"/>
       <c r="B49" s="2" t="s">
         <v>91</v>
       </c>
@@ -1905,14 +3371,24 @@
       <c r="D49" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
+      <c r="E49" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="9"/>
+      <c r="A50" s="10"/>
       <c r="B50" s="2" t="s">
         <v>93</v>
       </c>
@@ -1922,14 +3398,24 @@
       <c r="D50" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
+      <c r="E50" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="9"/>
+      <c r="A51" s="10"/>
       <c r="B51" s="2" t="s">
         <v>94</v>
       </c>
@@ -1939,14 +3425,24 @@
       <c r="D51" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="9"/>
+      <c r="A52" s="10"/>
       <c r="B52" s="2" t="s">
         <v>95</v>
       </c>
@@ -1956,14 +3452,24 @@
       <c r="D52" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="9"/>
+      <c r="A53" s="10"/>
       <c r="B53" s="2" t="s">
         <v>96</v>
       </c>
@@ -1973,14 +3479,24 @@
       <c r="D53" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
+      <c r="E53" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="9"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="2" t="s">
         <v>97</v>
       </c>
@@ -1990,14 +3506,24 @@
       <c r="D54" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
+      <c r="E54" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="9"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="2" t="s">
         <v>98</v>
       </c>
@@ -2007,14 +3533,24 @@
       <c r="D55" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
+      <c r="E55" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="9"/>
+      <c r="A56" s="10"/>
       <c r="B56" s="2" t="s">
         <v>99</v>
       </c>
@@ -2024,14 +3560,24 @@
       <c r="D56" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
+      <c r="E56" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="10" t="s">
         <v>178</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -2043,14 +3589,24 @@
       <c r="D57" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
+      <c r="E57" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="9"/>
+      <c r="A58" s="10"/>
       <c r="B58" s="2" t="s">
         <v>102</v>
       </c>
@@ -2060,14 +3616,24 @@
       <c r="D58" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
+      <c r="E58" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="9"/>
+      <c r="A59" s="10"/>
       <c r="B59" s="2" t="s">
         <v>104</v>
       </c>
@@ -2077,14 +3643,24 @@
       <c r="D59" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
+      <c r="E59" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="9"/>
+      <c r="A60" s="10"/>
       <c r="B60" s="2" t="s">
         <v>106</v>
       </c>
@@ -2094,14 +3670,24 @@
       <c r="D60" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
+      <c r="E60" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="9"/>
+      <c r="A61" s="10"/>
       <c r="B61" s="2" t="s">
         <v>108</v>
       </c>
@@ -2111,14 +3697,24 @@
       <c r="D61" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E61" s="2"/>
-      <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
+      <c r="E61" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="9"/>
+      <c r="A62" s="10"/>
       <c r="B62" s="2" t="s">
         <v>110</v>
       </c>
@@ -2128,14 +3724,24 @@
       <c r="D62" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
+      <c r="E62" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>498</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="9"/>
+      <c r="A63" s="10"/>
       <c r="B63" s="2" t="s">
         <v>112</v>
       </c>
@@ -2145,14 +3751,24 @@
       <c r="D63" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
+      <c r="E63" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>499</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="9"/>
+      <c r="A64" s="10"/>
       <c r="B64" s="2" t="s">
         <v>114</v>
       </c>
@@ -2162,14 +3778,24 @@
       <c r="D64" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>500</v>
+      </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="9"/>
+      <c r="A65" s="10"/>
       <c r="B65" s="2" t="s">
         <v>116</v>
       </c>
@@ -2179,14 +3805,24 @@
       <c r="D65" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
+      <c r="E65" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>501</v>
+      </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="9"/>
+      <c r="A66" s="10"/>
       <c r="B66" s="2" t="s">
         <v>118</v>
       </c>
@@ -2196,14 +3832,24 @@
       <c r="D66" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
+      <c r="E66" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>502</v>
+      </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="9"/>
+      <c r="A67" s="10"/>
       <c r="B67" s="2" t="s">
         <v>120</v>
       </c>
@@ -2213,14 +3859,24 @@
       <c r="D67" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
+      <c r="E67" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>503</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="9"/>
+      <c r="A68" s="10"/>
       <c r="B68" s="2" t="s">
         <v>122</v>
       </c>
@@ -2230,14 +3886,24 @@
       <c r="D68" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
+      <c r="E68" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>504</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="9"/>
+      <c r="A69" s="10"/>
       <c r="B69" s="2" t="s">
         <v>124</v>
       </c>
@@ -2247,14 +3913,24 @@
       <c r="D69" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-      <c r="I69" s="2"/>
+      <c r="E69" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="9"/>
+      <c r="A70" s="10"/>
       <c r="B70" s="2" t="s">
         <v>126</v>
       </c>
@@ -2264,14 +3940,18 @@
       <c r="D70" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
+      <c r="E70" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="9"/>
+      <c r="A71" s="10"/>
       <c r="B71" s="2" t="s">
         <v>128</v>
       </c>
@@ -2281,14 +3961,24 @@
       <c r="D71" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
+      <c r="E71" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>506</v>
+      </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="9"/>
+      <c r="A72" s="10"/>
       <c r="B72" s="2" t="s">
         <v>130</v>
       </c>
@@ -2298,14 +3988,24 @@
       <c r="D72" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-      <c r="I72" s="2"/>
+      <c r="E72" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>507</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="9"/>
+      <c r="A73" s="10"/>
       <c r="B73" s="2" t="s">
         <v>132</v>
       </c>
@@ -2315,14 +4015,24 @@
       <c r="D73" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E73" s="2"/>
-      <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
+      <c r="E73" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="9"/>
+      <c r="A74" s="10"/>
       <c r="B74" s="2" t="s">
         <v>134</v>
       </c>
@@ -2332,14 +4042,24 @@
       <c r="D74" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
+      <c r="E74" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="9" t="s">
+      <c r="A75" s="10" t="s">
         <v>177</v>
       </c>
       <c r="B75" s="2" t="s">
@@ -2351,14 +4071,24 @@
       <c r="D75" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="E75" s="2"/>
-      <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-      <c r="I75" s="2"/>
+      <c r="E75" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>510</v>
+      </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="9"/>
+      <c r="A76" s="10"/>
       <c r="B76" s="2" t="s">
         <v>138</v>
       </c>
@@ -2368,14 +4098,24 @@
       <c r="D76" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E76" s="2"/>
-      <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-      <c r="I76" s="2"/>
+      <c r="E76" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="9"/>
+      <c r="A77" s="10"/>
       <c r="B77" s="2" t="s">
         <v>140</v>
       </c>
@@ -2385,14 +4125,24 @@
       <c r="D77" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
+      <c r="E77" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="9"/>
+      <c r="A78" s="10"/>
       <c r="B78" s="2" t="s">
         <v>142</v>
       </c>
@@ -2402,14 +4152,24 @@
       <c r="D78" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="E78" s="2"/>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-      <c r="I78" s="2"/>
+      <c r="E78" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="9"/>
+      <c r="A79" s="10"/>
       <c r="B79" s="2" t="s">
         <v>144</v>
       </c>
@@ -2419,14 +4179,24 @@
       <c r="D79" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
+      <c r="E79" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="9"/>
+      <c r="A80" s="10"/>
       <c r="B80" s="2" t="s">
         <v>146</v>
       </c>
@@ -2436,14 +4206,24 @@
       <c r="D80" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
+      <c r="E80" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="9"/>
+      <c r="A81" s="10"/>
       <c r="B81" s="2" t="s">
         <v>148</v>
       </c>
@@ -2453,14 +4233,24 @@
       <c r="D81" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E81" s="2"/>
-      <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
+      <c r="E81" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="9"/>
+      <c r="A82" s="10"/>
       <c r="B82" s="2" t="s">
         <v>150</v>
       </c>
@@ -2470,14 +4260,24 @@
       <c r="D82" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-      <c r="I82" s="2"/>
+      <c r="E82" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>517</v>
+      </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="9"/>
+      <c r="A83" s="10"/>
       <c r="B83" s="2" t="s">
         <v>152</v>
       </c>
@@ -2487,14 +4287,24 @@
       <c r="D83" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="E83" s="2"/>
-      <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
+      <c r="E83" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>518</v>
+      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="9"/>
+      <c r="A84" s="10"/>
       <c r="B84" s="2" t="s">
         <v>154</v>
       </c>
@@ -2504,14 +4314,24 @@
       <c r="D84" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-      <c r="I84" s="2"/>
+      <c r="E84" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="9"/>
+      <c r="A85" s="10"/>
       <c r="B85" s="2" t="s">
         <v>156</v>
       </c>
@@ -2521,14 +4341,24 @@
       <c r="D85" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E85" s="2"/>
-      <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-      <c r="I85" s="2"/>
+      <c r="E85" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>520</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="9"/>
+      <c r="A86" s="10"/>
       <c r="B86" s="2" t="s">
         <v>158</v>
       </c>
@@ -2538,14 +4368,24 @@
       <c r="D86" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="2"/>
+      <c r="E86" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>521</v>
+      </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="9"/>
+      <c r="A87" s="10"/>
       <c r="B87" s="2" t="s">
         <v>160</v>
       </c>
@@ -2555,14 +4395,24 @@
       <c r="D87" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-      <c r="I87" s="2"/>
+      <c r="E87" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="9"/>
+      <c r="A88" s="10"/>
       <c r="B88" s="2" t="s">
         <v>162</v>
       </c>
@@ -2572,14 +4422,24 @@
       <c r="D88" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E88" s="2"/>
-      <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-      <c r="I88" s="2"/>
+      <c r="E88" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="9"/>
+      <c r="A89" s="10"/>
       <c r="B89" s="2" t="s">
         <v>164</v>
       </c>
@@ -2589,14 +4449,24 @@
       <c r="D89" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
+      <c r="E89" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="H89" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>524</v>
+      </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="9"/>
+      <c r="A90" s="10"/>
       <c r="B90" s="2" t="s">
         <v>166</v>
       </c>
@@ -2606,11 +4476,21 @@
       <c r="D90" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E90" s="2"/>
-      <c r="F90" s="2"/>
-      <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
+      <c r="E90" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>525</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>